<commit_message>
added bytes primitive type
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>struct</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>[float,float,float?]</t>
+  </si>
+  <si>
+    <t>If I make SEMANTIC a new structured field than I actually add 7 more reserved structures. Might be good while I think through fixed-list. Otherwise it's a wasted bit?</t>
+  </si>
+  <si>
+    <t>Semantic IDs using byte 2 would start at 256 in value and go up. uuid right now takes the first position</t>
+  </si>
+  <si>
+    <t>bytes</t>
   </si>
 </sst>
 </file>
@@ -179,13 +188,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -469,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" ref="P5:P6" si="0">128+O5 + (256*N5)</f>
+        <f t="shared" ref="P5" si="0">128+O5 + (256*N5)</f>
         <v>389</v>
       </c>
       <c r="Q5" s="3"/>
@@ -846,7 +856,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1389,6 +1399,16 @@
         <v>128</v>
       </c>
     </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
removed 'any' identifier type as it was complicated and not clearly valuable.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>struct</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>boolean</t>
-  </si>
-  <si>
-    <t>any</t>
   </si>
   <si>
     <t>geo</t>
@@ -482,7 +479,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +490,7 @@
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -505,7 +502,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="4"/>
@@ -520,7 +517,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -587,19 +584,19 @@
         <v>128</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -610,7 +607,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -633,21 +630,21 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <f>J21+J9</f>
-        <v>37</v>
+        <f>J21+J8</f>
+        <v>36</v>
       </c>
       <c r="P4" s="3">
         <f>128+O4+(256*N4)</f>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -658,7 +655,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -690,12 +687,12 @@
         <v>1</v>
       </c>
       <c r="O5" s="3">
-        <f>J9</f>
-        <v>5</v>
+        <f>J8</f>
+        <v>4</v>
       </c>
       <c r="P5" s="3">
         <f t="shared" ref="P5" si="0">128+O5 + (256*N5)</f>
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
@@ -706,7 +703,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -729,21 +726,21 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N6" s="3">
         <v>2</v>
       </c>
       <c r="O6" s="3">
-        <f>J20+J8</f>
-        <v>20</v>
+        <f>J20+J7</f>
+        <v>19</v>
       </c>
       <c r="P6" s="3">
         <f>128+O6+(256*N6)</f>
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -754,7 +751,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -788,7 +785,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -822,7 +819,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -856,7 +853,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1228,7 +1225,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1249,7 +1246,7 @@
         <v>32</v>
       </c>
       <c r="K21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1382,7 +1379,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1401,12 +1398,12 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remved 'fixed-list' type and clarified pass-through semantic identifiers.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>struct</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Byte 2</t>
-  </si>
-  <si>
-    <t>fixed-list</t>
   </si>
   <si>
     <t>SEMANTIC</t>
@@ -479,7 +476,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +514,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -584,19 +581,19 @@
         <v>128</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -630,10 +627,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -729,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N6" s="3">
         <v>2</v>
@@ -819,7 +816,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1225,7 +1222,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1246,7 +1243,7 @@
         <v>32</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1260,7 +1257,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1379,7 +1376,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1398,12 +1395,12 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Base-32 spec. Updated types spreadsheet to describe uuid correctly.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32920" windowHeight="19180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="32920" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>struct</t>
   </si>
@@ -89,12 +89,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>[long, long]</t>
-  </si>
-  <si>
-    <t>** Do I need to specify array size?</t>
-  </si>
-  <si>
     <t>type value</t>
   </si>
   <si>
@@ -104,19 +98,16 @@
     <t>[float,float,float?]</t>
   </si>
   <si>
-    <t>If I make SEMANTIC a new structured field than I actually add 7 more reserved structures. Might be good while I think through fixed-list. Otherwise it's a wasted bit?</t>
-  </si>
-  <si>
-    <t>Semantic IDs using byte 2 would start at 256 in value and go up. uuid right now takes the first position</t>
-  </si>
-  <si>
     <t>bytes</t>
+  </si>
+  <si>
+    <t>[16 bytes]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -205,6 +196,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -472,11 +466,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,10 +584,10 @@
         <v>18</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -630,18 +624,18 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <f>J21+J8</f>
-        <v>36</v>
+        <f>J9</f>
+        <v>5</v>
       </c>
       <c r="P4" s="3">
         <f>128+O4+(256*N4)</f>
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -726,7 +720,7 @@
         <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N6" s="3">
         <v>2</v>
@@ -816,7 +810,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1242,9 +1236,6 @@
         <f>(B21*B3)+(C21*C3)+(D21*D3)+(E21*E3)+(F21*F3)+(G21*G3)+(H21*H3)+(I21*I3)</f>
         <v>32</v>
       </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -1394,14 +1385,10 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More Geo clarity and added list-of types
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/spec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Projects/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32920" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>struct</t>
   </si>
@@ -95,19 +95,25 @@
     <t>total type</t>
   </si>
   <si>
-    <t>[float,float,float?]</t>
-  </si>
-  <si>
     <t>bytes</t>
   </si>
   <si>
     <t>[16 bytes]</t>
+  </si>
+  <si>
+    <t>[float,float]</t>
+  </si>
+  <si>
+    <t>list-of-lists</t>
+  </si>
+  <si>
+    <t>list-of-maps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -466,11 +472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,7 +630,7 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -720,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N6" s="3">
         <v>2</v>
@@ -810,7 +816,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1255,18 +1261,18 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22">
         <f>(B22*B3)+(C22*C3)+(D22*D3)+(E22*E3)+(F22*F3)+(G22*G3)+(H22*H3)+(I22*I3)</f>
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -1287,7 +1293,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1298,7 +1304,7 @@
       <c r="I23" s="1"/>
       <c r="J23">
         <f>(B23*B3)+(C23*C3)+(D23*D3)+(E23*E3)+(F23*F3)+(G23*G3)+(H23*H3)+(I23*I3)</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -1312,17 +1318,17 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -1330,7 +1336,7 @@
       <c r="I24" s="1"/>
       <c r="J24">
         <f>(B24*B3)+(C24*C3)+(D24*D3)+(E24*E3)+(F24*F3)+(G24*G3)+(H24*H3)+(I24*I3)</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -1344,14 +1350,14 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -1362,33 +1368,65 @@
       <c r="I25" s="1"/>
       <c r="J25">
         <f>(B25*B3)+(C25*C3)+(D25*D3)+(E25*E3)+(F25*F3)+(G25*G3)+(H25*H3)+(I25*I3)</f>
-        <v>112</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1">
-        <v>1</v>
-      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1"/>
       <c r="J26">
         <f>(B26*B3)+(C26*C3)+(D26*D3)+(E26*E3)+(F26*F3)+(G26*G3)+(H26*H3)+(I26*I3)</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f>(B27*B3)+(C27*C3)+(D27*D3)+(E27*E3)+(F27*F3)+(G27*G3)+(H27*H3)+(I27*I3)</f>
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-    </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved structural types down a slot.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Projects/Identifiers/spec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934924E6-9F11-DB4F-95A3-FDF2D7A3CF5B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>struct</t>
   </si>
@@ -108,12 +109,15 @@
   </si>
   <si>
     <t>list-of-maps</t>
+  </si>
+  <si>
+    <t>list-of</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -472,11 +476,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,12 +736,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="3">
-        <f>J20+J7</f>
-        <v>19</v>
+        <f>J7+J12</f>
+        <v>11</v>
       </c>
       <c r="P6" s="3">
         <f>128+O6+(256*N6)</f>
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -918,22 +922,20 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12">
@@ -952,27 +954,25 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13">
         <f>(B13*B3)+(C13*C3)+(D13*D3)+(E13*E3)+(F13*F3)+(G13*G3)+(H13*H3)+(I13*I3)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -988,25 +988,23 @@
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14">
         <f>(B14*B3)+(C14*C3)+(D14*D3)+(E14*E3)+(F14*F3)+(G14*G3)+(H14*H3)+(I14*I3)</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -1020,27 +1018,25 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15">
         <f>(B15*B3)+(C15*C3)+(D15*D3)+(E15*E3)+(F15*F3)+(G15*G3)+(H15*H3)+(I15*I3)</f>
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -1054,27 +1050,25 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16">
         <f>(B16*B3)+(C16*C3)+(D16*D3)+(E16*E3)+(F16*F3)+(G16*G3)+(H16*H3)+(I16*I3)</f>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -1088,27 +1082,25 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17">
         <f>(B17*B3)+(C17*C3)+(D17*D3)+(E17*E3)+(F17*F3)+(G17*G3)+(H17*H3)+(I17*I3)</f>
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1124,25 +1116,23 @@
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18">
         <f>(B18*B3)+(C18*C3)+(D18*D3)+(E18*E3)+(F18*F3)+(G18*G3)+(H18*H3)+(I18*I3)</f>
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -1158,25 +1148,19 @@
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19">
         <f>(B19*B3)+(C19*C3)+(D19*D3)+(E19*E3)+(F19*F3)+(G19*G3)+(H19*H3)+(I19*I3)</f>
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1190,25 +1174,19 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20">
         <f>(B20*B3)+(C20*C3)+(D20*D3)+(E20*E3)+(F20*F3)+(G20*G3)+(H20*H3)+(I20*I3)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1222,25 +1200,19 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21">
         <f>(B21*B3)+(C21*C3)+(D21*D3)+(E21*E3)+(F21*F3)+(G21*G3)+(H21*H3)+(I21*I3)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -1260,19 +1232,13 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22">
         <f>(B22*B3)+(C22*C3)+(D22*D3)+(E22*E3)+(F22*F3)+(G22*G3)+(H22*H3)+(I22*I3)</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -1292,19 +1258,13 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23">
         <f>(B23*B3)+(C23*C3)+(D23*D3)+(E23*E3)+(F23*F3)+(G23*G3)+(H23*H3)+(I23*I3)</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -1318,25 +1278,19 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
-      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24">
         <f>(B24*B3)+(C24*C3)+(D24*D3)+(E24*E3)+(F24*F3)+(G24*G3)+(H24*H3)+(I24*I3)</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -1350,25 +1304,19 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25">
         <f>(B25*B3)+(C25*C3)+(D25*D3)+(E25*E3)+(F25*F3)+(G25*G3)+(H25*H3)+(I25*I3)</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -1388,19 +1336,13 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26">
         <f>(B26*B3)+(C26*C3)+(D26*D3)+(E26*E3)+(F26*F3)+(G26*G3)+(H26*H3)+(I26*I3)</f>
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added lots of information to spec, including MsgPack details and type specs.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934924E6-9F11-DB4F-95A3-FDF2D7A3CF5B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD635E-106D-074A-81D0-09FECB598C9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>struct</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>list-of</t>
+  </si>
+  <si>
+    <t>semantic</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +544,9 @@
       <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
@@ -692,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" ref="P5" si="0">128+O5 + (256*N5)</f>
+        <f>128+O5 + (256*N5)</f>
         <v>388</v>
       </c>
       <c r="Q5" s="3"/>

</xml_diff>

<commit_message>
Changed concept of structured identifiers from something standalone to 'variants' of single identifiers. Added lots of detail on calculating type codes.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD635E-106D-074A-81D0-09FECB598C9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE0364D-4A18-4E48-A69C-AE57F5AF9104}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32060" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="P4" s="3">
-        <f>128+O4+(256*N4)</f>
+        <f>J27+O4+(256*N4)</f>
         <v>133</v>
       </c>
       <c r="Q4" s="3"/>
@@ -697,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="3">
-        <f>128+O5 + (256*N5)</f>
+        <f>J27+O5 + (256*N5)</f>
         <v>388</v>
       </c>
       <c r="Q5" s="3"/>
@@ -745,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="P6" s="3">
-        <f>128+O6+(256*N6)</f>
+        <f>J27+O6+(256*N6)</f>
         <v>651</v>
       </c>
       <c r="Q6" s="3"/>

</xml_diff>

<commit_message>
Add Composite IDs to tck. Changed tck fields "base128"/"base32" to "data"/"human" to match spec descriptions more clearly.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbishop/Sides/Identifiers/spec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Projects/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE0364D-4A18-4E48-A69C-AE57F5AF9104}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD584FF-3549-254C-A401-0A4EB157C4F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32060" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>struct</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>semantic</t>
+  </si>
+  <si>
+    <t>composite</t>
+  </si>
+  <si>
+    <t>composite-list</t>
+  </si>
+  <si>
+    <t>composite-map</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,12 +1037,8 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1">
         <v>1</v>
       </c>
@@ -1151,7 +1156,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1179,19 +1184,27 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20">
         <f>(B20*B3)+(C20*C3)+(D20*D3)+(E20*E3)+(F20*F3)+(G20*G3)+(H20*H3)+(I20*I3)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -1205,19 +1218,27 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21">
         <f>(B21*B3)+(C21*C3)+(D21*D3)+(E21*E3)+(F21*F3)+(G21*G3)+(H21*H3)+(I21*I3)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>

</xml_diff>

<commit_message>
Draft 2 changes: * Add map-of (similar to list-of) flag to support map-of-list and map-of-map identifier types. The geo semantic identifier has an example. * Moved composite-list and composite-map flags to new locations to accommodate map-of. * Regenerated TCK files with new format. * Added min and max long values.
</commit_message>
<xml_diff>
--- a/types.xlsx
+++ b/types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Projects/Identifiers/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD584FF-3549-254C-A401-0A4EB157C4F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2561FF6-B4D1-BB40-A918-3016D3039ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>struct</t>
   </si>
@@ -117,13 +117,25 @@
     <t>semantic</t>
   </si>
   <si>
-    <t>composite</t>
-  </si>
-  <si>
     <t>composite-list</t>
   </si>
   <si>
     <t>composite-map</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>map-of</t>
+  </si>
+  <si>
+    <t>map-of-list</t>
+  </si>
+  <si>
+    <t>map-of-map</t>
+  </si>
+  <si>
+    <t>COMPOSITE</t>
   </si>
 </sst>
 </file>
@@ -492,7 +504,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,8 +801,6 @@
         <v>3</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -856,6 +866,9 @@
         <f>(B9*B3)+(C9*C3)+(D9*D3)+(E9*E3)+(F9*F3)+(G9*G3)+(H9*H3)+(I9*I3)</f>
         <v>5</v>
       </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -947,9 +960,7 @@
       <c r="F12" s="1">
         <v>0</v>
       </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12">
@@ -979,9 +990,7 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13">
@@ -1000,7 +1009,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1011,9 +1020,7 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14">
@@ -1124,7 +1131,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1156,7 +1163,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1184,7 +1191,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1195,9 +1202,7 @@
       <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1">
         <v>1</v>
       </c>
@@ -1218,7 +1223,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1229,9 +1234,7 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="1">
         <v>1</v>
       </c>
@@ -1252,19 +1255,25 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22">
         <f>(B22*B3)+(C22*C3)+(D22*D3)+(E22*E3)+(F22*F3)+(G22*G3)+(H22*H3)+(I22*I3)</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>

</xml_diff>